<commit_message>
added adiabatic mixing to the overall jupyter
</commit_message>
<xml_diff>
--- a/Matrices ModelRecAir.xlsx
+++ b/Matrices ModelRecAir.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leni\Nextcloud\Lena\ZHAW\22 FS\EVA_DSH\EVA_DSH\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{758F26DE-906C-41AC-894A-87D08A3FEF49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23AF9E2D-CEAF-4213-833E-F67D7277D375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16956" yWindow="4116" windowWidth="11544" windowHeight="12480" xr2:uid="{9A57FA78-001C-43EB-8464-8033951E1EBB}"/>
+    <workbookView xWindow="11496" yWindow="24" windowWidth="11544" windowHeight="12480" xr2:uid="{9A57FA78-001C-43EB-8464-8033951E1EBB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="63">
   <si>
     <t>mc</t>
   </si>
@@ -254,6 +254,9 @@
   </si>
   <si>
     <t>w7</t>
+  </si>
+  <si>
+    <t>mama A</t>
   </si>
 </sst>
 </file>
@@ -632,8 +635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{701DF88A-65D7-4165-A88E-01FAFF2E9C69}">
   <dimension ref="A1:Z88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2182,7 +2185,7 @@
     <row r="64" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="65" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B65" s="3" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C65">
         <v>0</v>

</xml_diff>

<commit_message>
ad_hum.py, ad_hum_HX.py and ad_hum_HXdry.py ready and cleaned up
</commit_message>
<xml_diff>
--- a/Matrices ModelRecAir.xlsx
+++ b/Matrices ModelRecAir.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leni\Nextcloud\Lena\ZHAW\22 FS\EVA_DSH\EVA_DSH\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA37142D-36ED-4A14-A420-478A054BCA22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD676E8A-025B-409A-B0AA-F3DB3B8BCA5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{9A57FA78-001C-43EB-8464-8033951E1EBB}"/>
+    <workbookView xWindow="7980" yWindow="3660" windowWidth="23040" windowHeight="12504" xr2:uid="{9A57FA78-001C-43EB-8464-8033951E1EBB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="753" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="796" uniqueCount="105">
   <si>
     <t>mc</t>
   </si>
@@ -298,9 +298,6 @@
     <t>psy..wsp(Θs0)</t>
   </si>
   <si>
-    <t>XH</t>
-  </si>
-  <si>
     <t>-(1-b)</t>
   </si>
   <si>
@@ -316,9 +313,6 @@
     <t>bΘ3</t>
   </si>
   <si>
-    <t>(1-b)mlw1</t>
-  </si>
-  <si>
     <t>psy..wsp(Θs0)-ws</t>
   </si>
   <si>
@@ -353,13 +347,61 @@
   </si>
   <si>
     <t>UA_HX</t>
+  </si>
+  <si>
+    <t>HX1</t>
+  </si>
+  <si>
+    <t>HX2</t>
+  </si>
+  <si>
+    <t>XC1</t>
+  </si>
+  <si>
+    <t>XC2</t>
+  </si>
+  <si>
+    <t>XM1</t>
+  </si>
+  <si>
+    <t>XM2</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>(1-b_HX)ml</t>
+  </si>
+  <si>
+    <t>-(1-b_HX)ml</t>
+  </si>
+  <si>
+    <t>psy.wsp(Θs0)</t>
+  </si>
+  <si>
+    <t>psy.wsp(Θ_so)Θ_so - psy.w(Θ_so,1)</t>
+  </si>
+  <si>
+    <r>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1-b)mlw3</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -401,6 +443,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -422,7 +477,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -430,6 +485,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -744,10 +803,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{701DF88A-65D7-4165-A88E-01FAFF2E9C69}">
-  <dimension ref="A1:BD89"/>
+  <dimension ref="A1:BE93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AM67" sqref="AM67"/>
+    <sheetView tabSelected="1" topLeftCell="AO39" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AT65" sqref="AT65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1654,10 +1713,10 @@
         <v>18</v>
       </c>
       <c r="AQ21" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="AS21" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="BA21">
         <v>1</v>
@@ -1727,10 +1786,10 @@
         <v>20</v>
       </c>
       <c r="AQ23" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="AS23" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="AU23">
         <v>1</v>
@@ -1803,16 +1862,16 @@
         <v>22</v>
       </c>
       <c r="AE25" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="AG25" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="AQ25" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="AS25" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="BA25">
         <v>2</v>
@@ -1898,10 +1957,10 @@
         <v>61</v>
       </c>
       <c r="AU26" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="AV26" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="AW26" t="s">
         <v>51</v>
@@ -2118,7 +2177,7 @@
         <v>-1</v>
       </c>
       <c r="AT31" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="32" spans="1:56" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -2157,10 +2216,10 @@
         <v>1</v>
       </c>
       <c r="AT32" s="5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="33" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="33" spans="1:57" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>8</v>
       </c>
@@ -2193,7 +2252,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="34" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:57" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>9</v>
       </c>
@@ -2222,16 +2281,16 @@
         <v>4</v>
       </c>
       <c r="AM34" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AO34" s="5">
         <v>1</v>
       </c>
       <c r="AT34" s="5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="35" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="35" spans="1:57" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>9</v>
       </c>
@@ -2269,7 +2328,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="36" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:57" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>10</v>
       </c>
@@ -2308,10 +2367,10 @@
         <v>2</v>
       </c>
       <c r="AT36" s="5" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="37" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="37" spans="1:57" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>10</v>
       </c>
@@ -2352,7 +2411,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="38" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:57" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>11</v>
       </c>
@@ -2372,7 +2431,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:57" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>11</v>
       </c>
@@ -2440,16 +2499,16 @@
         <v>61</v>
       </c>
       <c r="AT39" t="s">
+        <v>83</v>
+      </c>
+      <c r="AU39" t="s">
+        <v>84</v>
+      </c>
+      <c r="AV39" t="s">
         <v>85</v>
       </c>
-      <c r="AU39" t="s">
+      <c r="AW39" t="s">
         <v>86</v>
-      </c>
-      <c r="AV39" t="s">
-        <v>87</v>
-      </c>
-      <c r="AW39" t="s">
-        <v>88</v>
       </c>
       <c r="AX39" t="s">
         <v>51</v>
@@ -2467,8 +2526,8 @@
         <v>67</v>
       </c>
     </row>
-    <row r="40" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="41" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:57" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="41" spans="1:57" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C41" t="s">
         <v>39</v>
       </c>
@@ -2578,8 +2637,8 @@
         <v>54</v>
       </c>
     </row>
-    <row r="42" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="43" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:57" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="1:57" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B43" s="3" t="s">
         <v>58</v>
       </c>
@@ -2644,7 +2703,7 @@
         <v>30</v>
       </c>
       <c r="AC43" s="3" t="s">
-        <v>58</v>
+        <v>28</v>
       </c>
       <c r="AD43">
         <v>0</v>
@@ -2706,14 +2765,26 @@
       <c r="AW43">
         <v>19</v>
       </c>
-      <c r="BA43" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="BC43" s="3" t="s">
+      <c r="AX43">
+        <v>20</v>
+      </c>
+      <c r="AY43">
+        <v>21</v>
+      </c>
+      <c r="AZ43">
+        <v>22</v>
+      </c>
+      <c r="BA43">
+        <v>23</v>
+      </c>
+      <c r="BB43">
+        <v>24</v>
+      </c>
+      <c r="BE43" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="44" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:57" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>1</v>
       </c>
@@ -2741,11 +2812,23 @@
       <c r="AC44">
         <v>0</v>
       </c>
-      <c r="AD44" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="45" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AE44">
+        <v>-1</v>
+      </c>
+      <c r="AG44">
+        <v>1</v>
+      </c>
+      <c r="BC44" t="s">
+        <v>63</v>
+      </c>
+      <c r="BD44">
+        <v>0</v>
+      </c>
+      <c r="BE44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:57" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>1</v>
       </c>
@@ -2773,8 +2856,26 @@
       <c r="AC45">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AD45" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF45" t="s">
+        <v>0</v>
+      </c>
+      <c r="AZ45">
+        <v>-1</v>
+      </c>
+      <c r="BC45" t="s">
+        <v>63</v>
+      </c>
+      <c r="BD45">
+        <v>1</v>
+      </c>
+      <c r="BE45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:57" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>59</v>
       </c>
@@ -2811,20 +2912,20 @@
       <c r="AF46" t="s">
         <v>0</v>
       </c>
-      <c r="AR46" s="1" t="s">
+      <c r="AP46" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="BA46" t="s">
-        <v>39</v>
-      </c>
-      <c r="BB46">
-        <v>0</v>
-      </c>
       <c r="BC46" t="s">
+        <v>1</v>
+      </c>
+      <c r="BD46">
+        <v>2</v>
+      </c>
+      <c r="BE46" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="47" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:57" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>59</v>
       </c>
@@ -2856,20 +2957,20 @@
       <c r="AG47" t="s">
         <v>3</v>
       </c>
-      <c r="AS47" s="1" t="s">
+      <c r="AQ47" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="BA47" t="s">
-        <v>40</v>
-      </c>
-      <c r="BB47">
-        <v>1</v>
-      </c>
       <c r="BC47" t="s">
+        <v>1</v>
+      </c>
+      <c r="BD47">
+        <v>3</v>
+      </c>
+      <c r="BE47" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="48" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:57" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>5</v>
       </c>
@@ -2895,34 +2996,31 @@
         <v>0</v>
       </c>
       <c r="AB48" t="s">
-        <v>59</v>
+        <v>5</v>
       </c>
       <c r="AC48">
         <v>4</v>
       </c>
       <c r="AF48" t="s">
-        <v>14</v>
-      </c>
-      <c r="AG48" s="1" t="s">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="AH48" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AI48" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="BA48" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="BB48">
-        <v>2</v>
-      </c>
-      <c r="BC48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+      <c r="AR48">
+        <v>1</v>
+      </c>
+      <c r="BC48" t="s">
+        <v>5</v>
+      </c>
+      <c r="BD48">
+        <v>4</v>
+      </c>
+      <c r="BE48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:57" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>5</v>
       </c>
@@ -2945,29 +3043,28 @@
         <v>0</v>
       </c>
       <c r="AB49" t="s">
-        <v>59</v>
+        <v>5</v>
       </c>
       <c r="AC49">
         <v>5</v>
       </c>
-      <c r="AG49" s="1"/>
-      <c r="AH49" t="s">
-        <v>57</v>
-      </c>
-      <c r="AI49">
-        <v>-1</v>
-      </c>
-      <c r="BA49" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="BB49">
+      <c r="AG49" t="s">
         <v>3</v>
       </c>
+      <c r="AI49" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="BC49" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="50" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="BD49">
+        <v>5</v>
+      </c>
+      <c r="BE49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:57" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>6</v>
       </c>
@@ -2996,31 +3093,34 @@
         <v>0</v>
       </c>
       <c r="AB50" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC50">
         <v>6</v>
       </c>
       <c r="AH50" t="s">
-        <v>0</v>
+        <v>14</v>
+      </c>
+      <c r="AI50" t="s">
+        <v>15</v>
       </c>
       <c r="AJ50" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="AT50">
-        <v>1</v>
-      </c>
-      <c r="BA50" t="s">
-        <v>43</v>
-      </c>
-      <c r="BB50">
-        <v>4</v>
-      </c>
-      <c r="BC50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+      <c r="AK50" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="BC50" t="s">
+        <v>6</v>
+      </c>
+      <c r="BD50">
+        <v>6</v>
+      </c>
+      <c r="BE50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:57" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>6</v>
       </c>
@@ -3043,28 +3143,28 @@
         <v>33</v>
       </c>
       <c r="AB51" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC51">
         <v>7</v>
       </c>
-      <c r="AI51" t="s">
-        <v>3</v>
-      </c>
-      <c r="AK51" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="BA51" t="s">
-        <v>44</v>
-      </c>
-      <c r="BB51">
-        <v>5</v>
-      </c>
-      <c r="BC51">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AJ51" t="s">
+        <v>18</v>
+      </c>
+      <c r="AK51">
+        <v>-1</v>
+      </c>
+      <c r="BC51" t="s">
+        <v>6</v>
+      </c>
+      <c r="BD51">
+        <v>7</v>
+      </c>
+      <c r="BE51" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="52" spans="1:57" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>7</v>
       </c>
@@ -3090,34 +3190,31 @@
         <v>0</v>
       </c>
       <c r="AB52" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AC52">
         <v>8</v>
       </c>
+      <c r="AH52" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="AJ52" t="s">
-        <v>14</v>
-      </c>
-      <c r="AK52" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="AL52" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AM52" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="BA52" t="s">
-        <v>45</v>
-      </c>
-      <c r="BB52">
-        <v>6</v>
-      </c>
-      <c r="BC52">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+      <c r="BC52" t="s">
+        <v>7</v>
+      </c>
+      <c r="BD52">
+        <v>8</v>
+      </c>
+      <c r="BE52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:57" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>7</v>
       </c>
@@ -3143,28 +3240,31 @@
         <v>0</v>
       </c>
       <c r="AB53" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AC53">
         <v>9</v>
       </c>
-      <c r="AL53" t="s">
-        <v>18</v>
-      </c>
-      <c r="AM53">
-        <v>-1</v>
-      </c>
-      <c r="BA53" t="s">
-        <v>46</v>
-      </c>
-      <c r="BB53">
+      <c r="AI53" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AK53" t="s">
+        <v>22</v>
+      </c>
+      <c r="AM53" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="BC53" t="s">
         <v>7</v>
       </c>
-      <c r="BC53" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="54" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="BD53">
+        <v>9</v>
+      </c>
+      <c r="BE53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:57" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>8</v>
       </c>
@@ -3190,31 +3290,31 @@
         <v>0</v>
       </c>
       <c r="AB54" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AC54">
         <v>10</v>
       </c>
-      <c r="AJ54" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="AL54" t="s">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="AN54" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="BA54" t="s">
-        <v>47</v>
-      </c>
-      <c r="BB54">
+      <c r="AS54">
+        <v>1</v>
+      </c>
+      <c r="BC54" t="s">
         <v>8</v>
       </c>
-      <c r="BC54">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="BD54">
+        <v>10</v>
+      </c>
+      <c r="BE54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:57" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>8</v>
       </c>
@@ -3237,31 +3337,28 @@
         <v>0</v>
       </c>
       <c r="AB55" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AC55">
         <v>11</v>
       </c>
-      <c r="AK55" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="AM55" t="s">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="AO55" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="BA55" t="s">
-        <v>48</v>
-      </c>
-      <c r="BB55">
-        <v>9</v>
-      </c>
-      <c r="BC55">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="BC55" t="s">
+        <v>8</v>
+      </c>
+      <c r="BD55">
+        <v>11</v>
+      </c>
+      <c r="BE55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:57" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>9</v>
       </c>
@@ -3287,7 +3384,7 @@
         <v>0</v>
       </c>
       <c r="AB56" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="AC56">
         <v>12</v>
@@ -3298,20 +3395,20 @@
       <c r="AP56" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="AU56">
-        <v>1</v>
-      </c>
-      <c r="BA56" t="s">
-        <v>49</v>
-      </c>
-      <c r="BB56">
-        <v>10</v>
-      </c>
-      <c r="BC56">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AT56">
+        <v>1</v>
+      </c>
+      <c r="BC56" t="s">
+        <v>9</v>
+      </c>
+      <c r="BD56">
+        <v>12</v>
+      </c>
+      <c r="BE56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:57" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>9</v>
       </c>
@@ -3337,7 +3434,7 @@
         <v>0</v>
       </c>
       <c r="AB57" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="AC57">
         <v>13</v>
@@ -3348,17 +3445,20 @@
       <c r="AQ57" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="BA57" t="s">
-        <v>50</v>
-      </c>
-      <c r="BB57">
-        <v>11</v>
-      </c>
-      <c r="BC57">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AU57">
+        <v>1</v>
+      </c>
+      <c r="BC57" t="s">
+        <v>9</v>
+      </c>
+      <c r="BD57">
+        <v>13</v>
+      </c>
+      <c r="BE57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:57" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>10</v>
       </c>
@@ -3381,31 +3481,28 @@
         <v>34</v>
       </c>
       <c r="AB58" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AC58">
         <v>14</v>
       </c>
       <c r="AP58" t="s">
-        <v>0</v>
-      </c>
-      <c r="AR58" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="AV58">
-        <v>1</v>
-      </c>
-      <c r="BA58" t="s">
-        <v>55</v>
-      </c>
-      <c r="BB58">
-        <v>12</v>
-      </c>
-      <c r="BC58">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+      <c r="AT58">
+        <v>1</v>
+      </c>
+      <c r="BC58" t="s">
+        <v>10</v>
+      </c>
+      <c r="BD58">
+        <v>14</v>
+      </c>
+      <c r="BE58" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="59" spans="1:57" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>10</v>
       </c>
@@ -3428,31 +3525,28 @@
         <v>35</v>
       </c>
       <c r="AB59" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AC59">
         <v>15</v>
       </c>
       <c r="AQ59" t="s">
-        <v>3</v>
-      </c>
-      <c r="AS59" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AW59">
-        <v>1</v>
-      </c>
-      <c r="BA59" t="s">
-        <v>56</v>
-      </c>
-      <c r="BB59">
-        <v>13</v>
-      </c>
-      <c r="BC59">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+      <c r="AU59">
+        <v>1</v>
+      </c>
+      <c r="BC59" t="s">
+        <v>10</v>
+      </c>
+      <c r="BD59">
+        <v>15</v>
+      </c>
+      <c r="BE59" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="60" spans="1:57" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>11</v>
       </c>
@@ -3475,28 +3569,28 @@
         <v>36</v>
       </c>
       <c r="AB60" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="AC60">
         <v>16</v>
       </c>
-      <c r="AR60" t="s">
-        <v>23</v>
-      </c>
-      <c r="AV60">
-        <v>1</v>
-      </c>
-      <c r="BA60" t="s">
-        <v>51</v>
-      </c>
-      <c r="BB60">
-        <v>14</v>
+      <c r="AP60" t="s">
+        <v>26</v>
+      </c>
+      <c r="AR60">
+        <v>1</v>
       </c>
       <c r="BC60" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="61" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+      <c r="BD60">
+        <v>16</v>
+      </c>
+      <c r="BE60" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="61" spans="1:57" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>11</v>
       </c>
@@ -3519,51 +3613,54 @@
         <v>37</v>
       </c>
       <c r="AB61" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="AC61">
         <v>17</v>
       </c>
-      <c r="AS61" t="s">
-        <v>24</v>
-      </c>
-      <c r="AW61">
-        <v>1</v>
-      </c>
-      <c r="BA61" t="s">
-        <v>52</v>
-      </c>
-      <c r="BB61">
-        <v>15</v>
+      <c r="AQ61" t="s">
+        <v>25</v>
+      </c>
+      <c r="AS61">
+        <v>1</v>
       </c>
       <c r="BC61" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="62" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+      <c r="BD61">
+        <v>17</v>
+      </c>
+      <c r="BE61" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="62" spans="1:57" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="AB62" t="s">
-        <v>11</v>
+        <v>64</v>
       </c>
       <c r="AC62">
         <v>18</v>
       </c>
+      <c r="AP62" s="1" t="s">
+        <v>88</v>
+      </c>
       <c r="AR62" t="s">
-        <v>26</v>
-      </c>
-      <c r="AT62">
-        <v>1</v>
-      </c>
-      <c r="BA62" t="s">
-        <v>53</v>
-      </c>
-      <c r="BB62">
-        <v>16</v>
+        <v>89</v>
+      </c>
+      <c r="BA62" s="9">
+        <v>1</v>
       </c>
       <c r="BC62" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="63" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+      <c r="BD62">
+        <v>18</v>
+      </c>
+      <c r="BE62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:57" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C63" t="s">
         <v>39</v>
       </c>
@@ -3619,42 +3716,57 @@
         <v>54</v>
       </c>
       <c r="AB63" t="s">
-        <v>11</v>
+        <v>64</v>
       </c>
       <c r="AC63">
         <v>19</v>
       </c>
-      <c r="AS63" t="s">
-        <v>25</v>
-      </c>
-      <c r="AU63">
-        <v>1</v>
-      </c>
-      <c r="BA63" t="s">
-        <v>54</v>
-      </c>
-      <c r="BB63">
-        <v>17</v>
+      <c r="AQ63" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="AS63" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="BB63" s="9">
+        <v>1</v>
       </c>
       <c r="BC63" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="64" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+      <c r="BD63">
+        <v>19</v>
+      </c>
+      <c r="BE63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:57" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="AB64" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AC64">
         <v>20</v>
       </c>
-      <c r="AT64" t="s">
-        <v>41</v>
-      </c>
-      <c r="AV64" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="65" spans="1:48" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AP64" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AR64" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AT64">
+        <v>1</v>
+      </c>
+      <c r="BC64" t="s">
+        <v>65</v>
+      </c>
+      <c r="BD64">
+        <v>20</v>
+      </c>
+      <c r="BE64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:57" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B65" s="3" t="s">
         <v>62</v>
       </c>
@@ -3719,19 +3831,33 @@
         <v>30</v>
       </c>
       <c r="AB65" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AC65">
         <v>21</v>
       </c>
-      <c r="AT65" t="s">
-        <v>42</v>
-      </c>
-      <c r="AV65" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="66" spans="1:48" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AQ65" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="AR65" s="9"/>
+      <c r="AS65" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="AT65" s="9"/>
+      <c r="AU65" s="9">
+        <v>1</v>
+      </c>
+      <c r="BC65" t="s">
+        <v>65</v>
+      </c>
+      <c r="BD65">
+        <v>21</v>
+      </c>
+      <c r="BE65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:57" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>1</v>
       </c>
@@ -3754,19 +3880,40 @@
         <v>31</v>
       </c>
       <c r="AB66" t="s">
-        <v>65</v>
+        <v>99</v>
       </c>
       <c r="AC66">
         <v>22</v>
       </c>
-      <c r="AT66" t="s">
-        <v>43</v>
-      </c>
-      <c r="AV66" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="67" spans="1:48" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AD66" t="s">
+        <v>92</v>
+      </c>
+      <c r="AF66" t="s">
+        <v>92</v>
+      </c>
+      <c r="AP66" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AR66" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="BA66" s="9">
+        <v>2</v>
+      </c>
+      <c r="BB66" s="9">
+        <v>2</v>
+      </c>
+      <c r="BC66" t="s">
+        <v>99</v>
+      </c>
+      <c r="BD66">
+        <v>22</v>
+      </c>
+      <c r="BE66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:57" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>1</v>
       </c>
@@ -3789,19 +3936,28 @@
         <v>32</v>
       </c>
       <c r="AB67" t="s">
-        <v>65</v>
+        <v>99</v>
       </c>
       <c r="AC67">
         <v>23</v>
       </c>
-      <c r="AT67" t="s">
-        <v>44</v>
-      </c>
-      <c r="AV67" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="68" spans="1:48" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AR67" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="AS67" s="9">
+        <v>-1</v>
+      </c>
+      <c r="BC67" t="s">
+        <v>99</v>
+      </c>
+      <c r="BD67">
+        <v>23</v>
+      </c>
+      <c r="BE67" s="9" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="68" spans="1:57" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>59</v>
       </c>
@@ -3830,13 +3986,31 @@
         <v>0</v>
       </c>
       <c r="AB68" t="s">
-        <v>67</v>
-      </c>
-      <c r="AV68" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="69" spans="1:48" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+      <c r="AC68">
+        <v>24</v>
+      </c>
+      <c r="AZ68">
+        <v>1</v>
+      </c>
+      <c r="BA68">
+        <v>-1</v>
+      </c>
+      <c r="BB68">
+        <v>-1</v>
+      </c>
+      <c r="BC68" t="s">
+        <v>99</v>
+      </c>
+      <c r="BD68">
+        <v>24</v>
+      </c>
+      <c r="BE68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:57" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>59</v>
       </c>
@@ -3859,11 +4033,86 @@
       <c r="Z69" t="s">
         <v>33</v>
       </c>
+      <c r="AC69" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD69" t="s">
+        <v>39</v>
+      </c>
+      <c r="AE69" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF69" t="s">
+        <v>41</v>
+      </c>
+      <c r="AG69" t="s">
+        <v>42</v>
+      </c>
+      <c r="AH69" t="s">
+        <v>43</v>
+      </c>
+      <c r="AI69" t="s">
+        <v>44</v>
+      </c>
+      <c r="AJ69" t="s">
+        <v>45</v>
+      </c>
+      <c r="AK69" t="s">
+        <v>46</v>
+      </c>
+      <c r="AL69" t="s">
+        <v>47</v>
+      </c>
+      <c r="AM69" t="s">
+        <v>48</v>
+      </c>
+      <c r="AN69" t="s">
+        <v>49</v>
+      </c>
+      <c r="AO69" t="s">
+        <v>50</v>
+      </c>
+      <c r="AP69" t="s">
+        <v>55</v>
+      </c>
+      <c r="AQ69" t="s">
+        <v>56</v>
+      </c>
+      <c r="AR69" t="s">
+        <v>60</v>
+      </c>
+      <c r="AS69" t="s">
+        <v>61</v>
+      </c>
+      <c r="AT69" t="s">
+        <v>83</v>
+      </c>
+      <c r="AU69" t="s">
+        <v>84</v>
+      </c>
       <c r="AV69" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="70" spans="1:48" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+      <c r="AW69" t="s">
+        <v>52</v>
+      </c>
+      <c r="AX69" t="s">
+        <v>53</v>
+      </c>
+      <c r="AY69" t="s">
+        <v>54</v>
+      </c>
+      <c r="AZ69" t="s">
+        <v>67</v>
+      </c>
+      <c r="BA69" t="s">
+        <v>72</v>
+      </c>
+      <c r="BB69" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="70" spans="1:57" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>5</v>
       </c>
@@ -3888,11 +4137,8 @@
       <c r="Z70">
         <v>0</v>
       </c>
-      <c r="AV70" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="71" spans="1:48" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="71" spans="1:57" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>5</v>
       </c>
@@ -3914,11 +4160,47 @@
       <c r="Z71">
         <v>0</v>
       </c>
-      <c r="AV71" t="s">
+      <c r="AD71" t="s">
+        <v>41</v>
+      </c>
+      <c r="AE71" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF71" t="s">
+        <v>43</v>
+      </c>
+      <c r="AG71" t="s">
+        <v>44</v>
+      </c>
+      <c r="AP71" t="s">
+        <v>45</v>
+      </c>
+      <c r="AQ71" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="72" spans="1:48" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AR71" t="s">
+        <v>68</v>
+      </c>
+      <c r="AS71" t="s">
+        <v>69</v>
+      </c>
+      <c r="AT71" t="s">
+        <v>47</v>
+      </c>
+      <c r="AU71" t="s">
+        <v>48</v>
+      </c>
+      <c r="AZ71" t="s">
+        <v>67</v>
+      </c>
+      <c r="BA71" t="s">
+        <v>72</v>
+      </c>
+      <c r="BB71" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="72" spans="1:57" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>6</v>
       </c>
@@ -3946,11 +4228,8 @@
       <c r="Z72">
         <v>0</v>
       </c>
-      <c r="AV72" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="73" spans="1:48" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="73" spans="1:57" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>6</v>
       </c>
@@ -3972,11 +4251,38 @@
       <c r="Z73" t="s">
         <v>33</v>
       </c>
-      <c r="AV73" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="74" spans="1:48" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AJ73">
+        <v>0</v>
+      </c>
+      <c r="AK73">
+        <v>1</v>
+      </c>
+      <c r="AL73">
+        <v>2</v>
+      </c>
+      <c r="AM73">
+        <v>3</v>
+      </c>
+      <c r="AN73">
+        <v>4</v>
+      </c>
+      <c r="AO73">
+        <v>5</v>
+      </c>
+      <c r="AP73">
+        <v>6</v>
+      </c>
+      <c r="AQ73">
+        <v>7</v>
+      </c>
+      <c r="AR73">
+        <v>8</v>
+      </c>
+      <c r="AT73" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="74" spans="1:57" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>7</v>
       </c>
@@ -4001,11 +4307,22 @@
       <c r="Z74">
         <v>0</v>
       </c>
-      <c r="AV74" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="75" spans="1:48" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AH74" t="s">
+        <v>93</v>
+      </c>
+      <c r="AI74">
+        <v>8</v>
+      </c>
+      <c r="AK74" s="5">
+        <v>1</v>
+      </c>
+      <c r="AM74" s="1"/>
+      <c r="AT74" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="AU74" s="7"/>
+    </row>
+    <row r="75" spans="1:57" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>7</v>
       </c>
@@ -4030,11 +4347,25 @@
       <c r="Z75">
         <v>0</v>
       </c>
-      <c r="AV75" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="76" spans="1:48" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AH75" t="s">
+        <v>94</v>
+      </c>
+      <c r="AI75">
+        <v>2</v>
+      </c>
+      <c r="AJ75" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN75" s="1"/>
+      <c r="AR75" s="5">
+        <v>-1</v>
+      </c>
+      <c r="AT75" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="AU75" s="7"/>
+    </row>
+    <row r="76" spans="1:57" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>27</v>
       </c>
@@ -4063,11 +4394,24 @@
       <c r="Z76">
         <v>0</v>
       </c>
-      <c r="AV76" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="77" spans="1:48" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AH76" t="s">
+        <v>95</v>
+      </c>
+      <c r="AI76">
+        <v>3</v>
+      </c>
+      <c r="AL76" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="AP76" s="5">
+        <v>1</v>
+      </c>
+      <c r="AT76" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="AU76" s="7"/>
+    </row>
+    <row r="77" spans="1:57" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>27</v>
       </c>
@@ -4091,11 +4435,24 @@
       <c r="Z77" t="s">
         <v>33</v>
       </c>
-      <c r="AV77" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="78" spans="1:48" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AH77" t="s">
+        <v>96</v>
+      </c>
+      <c r="AI77">
+        <v>4</v>
+      </c>
+      <c r="AM77" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="AQ77" s="5">
+        <v>1</v>
+      </c>
+      <c r="AT77" t="s">
+        <v>104</v>
+      </c>
+      <c r="AU77" s="7"/>
+    </row>
+    <row r="78" spans="1:57" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>8</v>
       </c>
@@ -4120,14 +4477,24 @@
       <c r="Z78">
         <v>0</v>
       </c>
-      <c r="AT78" t="s">
-        <v>45</v>
-      </c>
-      <c r="AV78" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="79" spans="1:48" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AH78" t="s">
+        <v>97</v>
+      </c>
+      <c r="AI78">
+        <v>6</v>
+      </c>
+      <c r="AL78" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="AN78" s="5">
+        <v>1</v>
+      </c>
+      <c r="AT78" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="AU78" s="7"/>
+    </row>
+    <row r="79" spans="1:57" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>8</v>
       </c>
@@ -4149,44 +4516,25 @@
       <c r="Z79">
         <v>0</v>
       </c>
-      <c r="AG79">
-        <v>0</v>
-      </c>
-      <c r="AH79">
-        <v>1</v>
+      <c r="AH79" t="s">
+        <v>98</v>
       </c>
       <c r="AI79">
-        <v>2</v>
-      </c>
-      <c r="AJ79">
-        <v>3</v>
-      </c>
-      <c r="AK79">
-        <v>4</v>
-      </c>
-      <c r="AL79">
-        <v>5</v>
-      </c>
-      <c r="AM79">
-        <v>6</v>
-      </c>
-      <c r="AN79">
         <v>7</v>
       </c>
-      <c r="AO79">
-        <v>8</v>
-      </c>
-      <c r="AP79" t="s">
-        <v>38</v>
-      </c>
-      <c r="AT79" t="s">
-        <v>46</v>
-      </c>
-      <c r="AV79" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="80" spans="1:48" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AM79" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="AN79" s="5"/>
+      <c r="AO79" s="5">
+        <v>1</v>
+      </c>
+      <c r="AT79" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="AU79" s="7"/>
+    </row>
+    <row r="80" spans="1:57" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>9</v>
       </c>
@@ -4211,36 +4559,30 @@
       <c r="Z80">
         <v>0</v>
       </c>
-      <c r="AE80" t="s">
-        <v>63</v>
-      </c>
-      <c r="AF80">
-        <v>0</v>
-      </c>
-      <c r="AI80" s="1"/>
-      <c r="AM80">
-        <v>-1</v>
-      </c>
-      <c r="AN80">
-        <v>-1</v>
-      </c>
-      <c r="AO80">
-        <v>1</v>
-      </c>
-      <c r="AP80" t="s">
-        <v>67</v>
-      </c>
-      <c r="AR80">
-        <v>0</v>
-      </c>
-      <c r="AT80" t="s">
-        <v>68</v>
-      </c>
-      <c r="AV80" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="81" spans="1:48" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AH80" t="s">
+        <v>99</v>
+      </c>
+      <c r="AI80">
+        <v>1</v>
+      </c>
+      <c r="AJ80" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="AL80" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="AP80" s="5">
+        <v>2</v>
+      </c>
+      <c r="AQ80" s="5">
+        <v>2</v>
+      </c>
+      <c r="AT80" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="AU80" s="7"/>
+    </row>
+    <row r="81" spans="1:46" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>9</v>
       </c>
@@ -4265,38 +4607,29 @@
       <c r="Z81">
         <v>0</v>
       </c>
-      <c r="AE81" t="s">
-        <v>63</v>
-      </c>
-      <c r="AF81">
-        <v>1</v>
-      </c>
-      <c r="AG81" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="AI81" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="AM81">
-        <v>2</v>
-      </c>
-      <c r="AN81">
-        <v>2</v>
-      </c>
-      <c r="AP81" t="s">
-        <v>43</v>
-      </c>
-      <c r="AR81" t="s">
-        <v>78</v>
-      </c>
-      <c r="AT81" t="s">
-        <v>69</v>
-      </c>
-      <c r="AV81" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="82" spans="1:48" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AH81" t="s">
+        <v>99</v>
+      </c>
+      <c r="AI81">
+        <v>5</v>
+      </c>
+      <c r="AL81" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AM81" s="5">
+        <v>-1</v>
+      </c>
+      <c r="AN81" s="5"/>
+      <c r="AO81" s="5"/>
+      <c r="AP81" s="5"/>
+      <c r="AQ81" s="5"/>
+      <c r="AR81" s="5"/>
+      <c r="AS81" s="5"/>
+      <c r="AT81" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="82" spans="1:46" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>10</v>
       </c>
@@ -4318,33 +4651,28 @@
       <c r="Z82" t="s">
         <v>34</v>
       </c>
-      <c r="AE82" t="s">
-        <v>76</v>
-      </c>
-      <c r="AF82">
-        <v>2</v>
-      </c>
-      <c r="AG82" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK82" s="1"/>
-      <c r="AO82">
+      <c r="AH82" t="s">
+        <v>99</v>
+      </c>
+      <c r="AI82">
+        <v>0</v>
+      </c>
+      <c r="AL82" s="1"/>
+      <c r="AP82" s="5">
         <v>-1</v>
       </c>
-      <c r="AP82" t="s">
-        <v>44</v>
-      </c>
-      <c r="AR82" t="s">
-        <v>79</v>
-      </c>
-      <c r="AT82" t="s">
-        <v>47</v>
-      </c>
-      <c r="AV82" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="83" spans="1:48" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AQ82" s="5">
+        <v>-1</v>
+      </c>
+      <c r="AR82" s="5">
+        <v>1</v>
+      </c>
+      <c r="AS82" s="5"/>
+      <c r="AT82" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:46" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>10</v>
       </c>
@@ -4366,32 +4694,38 @@
       <c r="Z83" t="s">
         <v>35</v>
       </c>
-      <c r="AE83" t="s">
-        <v>64</v>
-      </c>
-      <c r="AF83">
-        <v>3</v>
-      </c>
-      <c r="AI83" t="s">
-        <v>73</v>
-      </c>
-      <c r="AM83">
-        <v>1</v>
+      <c r="AC83" t="s">
+        <v>63</v>
+      </c>
+      <c r="AJ83" t="s">
+        <v>43</v>
+      </c>
+      <c r="AK83" t="s">
+        <v>44</v>
+      </c>
+      <c r="AL83" t="s">
+        <v>68</v>
+      </c>
+      <c r="AM83" t="s">
+        <v>69</v>
+      </c>
+      <c r="AN83" t="s">
+        <v>47</v>
+      </c>
+      <c r="AO83" t="s">
+        <v>48</v>
       </c>
       <c r="AP83" t="s">
-        <v>68</v>
+        <v>72</v>
+      </c>
+      <c r="AQ83" t="s">
+        <v>71</v>
       </c>
       <c r="AR83" t="s">
-        <v>80</v>
-      </c>
-      <c r="AT83" t="s">
-        <v>48</v>
-      </c>
-      <c r="AV83" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="84" spans="1:48" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="84" spans="1:46" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>11</v>
       </c>
@@ -4413,29 +4747,11 @@
       <c r="Z84" t="s">
         <v>36</v>
       </c>
-      <c r="AE84" t="s">
-        <v>64</v>
-      </c>
-      <c r="AF84">
-        <v>4</v>
-      </c>
-      <c r="AJ84" t="s">
-        <v>74</v>
-      </c>
-      <c r="AN84">
-        <v>1</v>
-      </c>
-      <c r="AP84" t="s">
-        <v>69</v>
-      </c>
-      <c r="AR84" t="s">
-        <v>82</v>
-      </c>
-      <c r="AV84" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="85" spans="1:48" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AC84" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="85" spans="1:46" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>11</v>
       </c>
@@ -4457,52 +4773,61 @@
       <c r="Z85" t="s">
         <v>37</v>
       </c>
-      <c r="AE85" t="s">
+      <c r="AC85" t="s">
         <v>64</v>
       </c>
-      <c r="AF85">
+      <c r="AJ85">
+        <v>0</v>
+      </c>
+      <c r="AK85">
+        <v>1</v>
+      </c>
+      <c r="AL85">
+        <v>2</v>
+      </c>
+      <c r="AM85">
+        <v>3</v>
+      </c>
+      <c r="AN85">
+        <v>4</v>
+      </c>
+      <c r="AO85">
         <v>5</v>
       </c>
-      <c r="AI85" t="s">
-        <v>75</v>
-      </c>
-      <c r="AJ85">
-        <v>-1</v>
-      </c>
-      <c r="AP85" t="s">
-        <v>47</v>
-      </c>
-      <c r="AR85" t="s">
-        <v>83</v>
-      </c>
-      <c r="AV85" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="86" spans="1:48" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="AE86" t="s">
-        <v>65</v>
-      </c>
-      <c r="AF86">
+      <c r="AP85">
         <v>6</v>
       </c>
-      <c r="AI86" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="AK86">
-        <v>1</v>
-      </c>
-      <c r="AP86" t="s">
-        <v>48</v>
-      </c>
-      <c r="AR86" t="s">
-        <v>81</v>
-      </c>
-      <c r="AV86" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="87" spans="1:48" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AT85" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="86" spans="1:46" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AC86" t="s">
+        <v>64</v>
+      </c>
+      <c r="AH86" t="s">
+        <v>63</v>
+      </c>
+      <c r="AI86">
+        <v>0</v>
+      </c>
+      <c r="AJ86" s="7"/>
+      <c r="AK86" s="7">
+        <v>1</v>
+      </c>
+      <c r="AL86" s="7"/>
+      <c r="AM86" s="7"/>
+      <c r="AN86" s="7"/>
+      <c r="AO86" s="7"/>
+      <c r="AP86" s="7"/>
+      <c r="AQ86" s="7"/>
+      <c r="AR86" s="7"/>
+      <c r="AS86" s="7"/>
+      <c r="AT86" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="87" spans="1:46" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C87" t="s">
         <v>39</v>
       </c>
@@ -4563,83 +4888,188 @@
       <c r="V87" t="s">
         <v>54</v>
       </c>
-      <c r="AE87" t="s">
+      <c r="AC87" t="s">
         <v>65</v>
       </c>
-      <c r="AF87">
-        <v>7</v>
-      </c>
-      <c r="AJ87" s="1" t="s">
+      <c r="AH87" t="s">
+        <v>63</v>
+      </c>
+      <c r="AI87">
+        <v>1</v>
+      </c>
+      <c r="AJ87" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="AK87" s="7"/>
+      <c r="AL87" s="7"/>
+      <c r="AM87" s="8"/>
+      <c r="AN87" s="7"/>
+      <c r="AO87" s="7"/>
+      <c r="AP87" s="8">
+        <v>-1</v>
+      </c>
+      <c r="AQ87" s="7"/>
+      <c r="AR87" s="7"/>
+      <c r="AS87" s="7"/>
+      <c r="AT87" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="88" spans="1:46" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AC88" t="s">
+        <v>65</v>
+      </c>
+      <c r="AH88" t="s">
+        <v>64</v>
+      </c>
+      <c r="AI88">
+        <v>2</v>
+      </c>
+      <c r="AJ88" s="7"/>
+      <c r="AK88" s="7"/>
+      <c r="AL88" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="AM88" s="7"/>
+      <c r="AN88" s="7"/>
+      <c r="AO88" s="7"/>
+      <c r="AP88" s="7">
+        <v>1</v>
+      </c>
+      <c r="AQ88" s="7"/>
+      <c r="AR88" s="7"/>
+      <c r="AS88" s="7"/>
+      <c r="AT88" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="89" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="AC89" t="s">
+        <v>67</v>
+      </c>
+      <c r="AH89" t="s">
+        <v>64</v>
+      </c>
+      <c r="AI89">
+        <v>3</v>
+      </c>
+      <c r="AJ89" s="7"/>
+      <c r="AK89" s="7"/>
+      <c r="AL89" s="7"/>
+      <c r="AM89" s="7">
+        <v>1</v>
+      </c>
+      <c r="AN89" s="7"/>
+      <c r="AO89" s="7"/>
+      <c r="AP89" s="7"/>
+      <c r="AQ89" s="7"/>
+      <c r="AR89" s="7"/>
+      <c r="AS89" s="7"/>
+      <c r="AT89" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="90" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="AH90" t="s">
+        <v>65</v>
+      </c>
+      <c r="AI90">
+        <v>4</v>
+      </c>
+      <c r="AJ90" s="7"/>
+      <c r="AK90" s="7"/>
+      <c r="AL90" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="AM90" s="7"/>
+      <c r="AN90" s="7">
+        <v>1</v>
+      </c>
+      <c r="AO90" s="7"/>
+      <c r="AP90" s="7"/>
+      <c r="AQ90" s="7"/>
+      <c r="AR90" s="7"/>
+      <c r="AS90" s="7"/>
+      <c r="AT90" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="91" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="AH91" t="s">
+        <v>65</v>
+      </c>
+      <c r="AI91">
+        <v>5</v>
+      </c>
+      <c r="AJ91" s="7"/>
+      <c r="AK91" s="7"/>
+      <c r="AL91" s="7"/>
+      <c r="AM91" s="7"/>
+      <c r="AN91" s="7"/>
+      <c r="AO91" s="7">
+        <v>1</v>
+      </c>
+      <c r="AP91" s="7"/>
+      <c r="AQ91" s="7"/>
+      <c r="AR91" s="7"/>
+      <c r="AS91" s="7"/>
+      <c r="AT91" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="92" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="AH92" t="s">
+        <v>67</v>
+      </c>
+      <c r="AI92">
+        <v>6</v>
+      </c>
+      <c r="AJ92" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="AK92" s="7"/>
+      <c r="AL92" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="AM92" s="7"/>
+      <c r="AN92" s="7"/>
+      <c r="AO92" s="7"/>
+      <c r="AP92" s="7">
+        <v>2</v>
+      </c>
+      <c r="AQ92" s="7"/>
+      <c r="AR92" s="7"/>
+      <c r="AS92" s="7"/>
+      <c r="AT92" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="AL87">
-        <v>1</v>
-      </c>
-      <c r="AP87" t="s">
-        <v>71</v>
-      </c>
-      <c r="AR87" t="s">
-        <v>84</v>
-      </c>
-      <c r="AV87" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="88" spans="1:48" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="AE88" t="s">
-        <v>65</v>
-      </c>
-      <c r="AF88">
-        <v>8</v>
-      </c>
-      <c r="AH88">
-        <v>1</v>
-      </c>
-      <c r="AJ88" s="1"/>
-      <c r="AP88" t="s">
-        <v>72</v>
-      </c>
-      <c r="AR88" t="s">
-        <v>42</v>
-      </c>
-      <c r="AT88" t="s">
-        <v>67</v>
-      </c>
-      <c r="AV88" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="89" spans="1:48" x14ac:dyDescent="0.3">
-      <c r="AG89" t="s">
+    </row>
+    <row r="93" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="AJ93" t="s">
         <v>43</v>
       </c>
-      <c r="AH89" t="s">
+      <c r="AK93" t="s">
         <v>44</v>
       </c>
-      <c r="AI89" t="s">
+      <c r="AL93" t="s">
         <v>68</v>
       </c>
-      <c r="AJ89" t="s">
+      <c r="AM93" t="s">
         <v>69</v>
       </c>
-      <c r="AK89" t="s">
+      <c r="AN93" t="s">
         <v>47</v>
       </c>
-      <c r="AL89" t="s">
+      <c r="AO93" t="s">
         <v>48</v>
       </c>
-      <c r="AM89" t="s">
-        <v>72</v>
-      </c>
-      <c r="AN89" t="s">
-        <v>71</v>
-      </c>
-      <c r="AO89" t="s">
+      <c r="AP93" t="s">
         <v>67</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Corrected A for mama and mxmx
</commit_message>
<xml_diff>
--- a/Matrices ModelRecAir.xlsx
+++ b/Matrices ModelRecAir.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ellio\Documents\GitHub\EVA_DSH\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{405F43A1-0307-4C86-B0F1-0E89C3D14CC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5BBA760-229F-447D-B0C3-410D1F59E154}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9A57FA78-001C-43EB-8464-8033951E1EBB}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="797" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1247" uniqueCount="117">
   <si>
     <t>mc</t>
   </si>
@@ -423,12 +423,21 @@
   <si>
     <t>-UA_HX*Θo</t>
   </si>
+  <si>
+    <t>m_i l w_0 + Q_la</t>
+  </si>
+  <si>
+    <t>Θ10</t>
+  </si>
+  <si>
+    <t>w10</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -483,6 +492,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -504,7 +528,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -516,6 +540,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -830,10 +856,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{701DF88A-65D7-4165-A88E-01FAFF2E9C69}">
-  <dimension ref="A1:BE93"/>
+  <dimension ref="A1:BE195"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z36" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="BE67" sqref="BE67"/>
+    <sheetView tabSelected="1" topLeftCell="A93" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AC107" sqref="AC107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -900,7 +926,7 @@
       <c r="X2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AD2" s="3" t="s">
+      <c r="AD2" s="12" t="s">
         <v>28</v>
       </c>
       <c r="AE2">
@@ -2729,7 +2755,7 @@
       <c r="X43" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AC43" s="3" t="s">
+      <c r="AC43" s="11" t="s">
         <v>28</v>
       </c>
       <c r="AD43">
@@ -3570,7 +3596,7 @@
         <v>15</v>
       </c>
       <c r="BE59" t="s">
-        <v>35</v>
+        <v>114</v>
       </c>
     </row>
     <row r="60" spans="1:57" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -5091,6 +5117,2783 @@
         <v>67</v>
       </c>
     </row>
+    <row r="99" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="C99" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D99">
+        <v>0</v>
+      </c>
+      <c r="E99">
+        <v>1</v>
+      </c>
+      <c r="F99">
+        <v>2</v>
+      </c>
+      <c r="G99">
+        <v>3</v>
+      </c>
+      <c r="H99">
+        <v>4</v>
+      </c>
+      <c r="I99">
+        <v>5</v>
+      </c>
+      <c r="J99">
+        <v>6</v>
+      </c>
+      <c r="K99">
+        <v>7</v>
+      </c>
+      <c r="L99">
+        <v>8</v>
+      </c>
+      <c r="M99">
+        <v>9</v>
+      </c>
+      <c r="N99">
+        <v>10</v>
+      </c>
+      <c r="O99">
+        <v>11</v>
+      </c>
+      <c r="P99">
+        <v>12</v>
+      </c>
+      <c r="Q99">
+        <v>13</v>
+      </c>
+      <c r="R99">
+        <v>14</v>
+      </c>
+      <c r="S99">
+        <v>15</v>
+      </c>
+      <c r="T99">
+        <v>16</v>
+      </c>
+      <c r="U99">
+        <v>17</v>
+      </c>
+      <c r="V99">
+        <v>18</v>
+      </c>
+      <c r="W99">
+        <v>19</v>
+      </c>
+      <c r="X99">
+        <v>20</v>
+      </c>
+      <c r="Y99">
+        <v>21</v>
+      </c>
+      <c r="Z99">
+        <v>22</v>
+      </c>
+      <c r="AA99">
+        <v>23</v>
+      </c>
+      <c r="AB99">
+        <v>24</v>
+      </c>
+      <c r="AC99">
+        <v>25</v>
+      </c>
+      <c r="AD99">
+        <v>26</v>
+      </c>
+      <c r="AG99" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="100" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="B100" t="s">
+        <v>63</v>
+      </c>
+      <c r="C100">
+        <v>0</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB100">
+        <v>1</v>
+      </c>
+      <c r="AE100" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF100">
+        <v>0</v>
+      </c>
+      <c r="AG100" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="101" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="B101" t="s">
+        <v>63</v>
+      </c>
+      <c r="C101">
+        <v>1</v>
+      </c>
+      <c r="E101">
+        <v>1</v>
+      </c>
+      <c r="AE101" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF101">
+        <v>1</v>
+      </c>
+      <c r="AG101" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="102" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="B102" t="s">
+        <v>1</v>
+      </c>
+      <c r="C102">
+        <v>2</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F102" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R102" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="AE102" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF102">
+        <v>2</v>
+      </c>
+      <c r="AG102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="B103" t="s">
+        <v>1</v>
+      </c>
+      <c r="C103">
+        <v>3</v>
+      </c>
+      <c r="E103" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G103" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="S103" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="AE103" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF103">
+        <v>3</v>
+      </c>
+      <c r="AG103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="B104" t="s">
+        <v>59</v>
+      </c>
+      <c r="C104">
+        <v>4</v>
+      </c>
+      <c r="F104" t="s">
+        <v>14</v>
+      </c>
+      <c r="G104" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H104" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I104" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AE104" t="s">
+        <v>59</v>
+      </c>
+      <c r="AF104">
+        <v>4</v>
+      </c>
+      <c r="AG104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="B105" t="s">
+        <v>59</v>
+      </c>
+      <c r="C105">
+        <v>5</v>
+      </c>
+      <c r="G105" s="1"/>
+      <c r="H105" t="s">
+        <v>57</v>
+      </c>
+      <c r="I105">
+        <v>-1</v>
+      </c>
+      <c r="AE105" t="s">
+        <v>59</v>
+      </c>
+      <c r="AF105">
+        <v>5</v>
+      </c>
+      <c r="AG105" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="106" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="B106" t="s">
+        <v>5</v>
+      </c>
+      <c r="C106">
+        <v>6</v>
+      </c>
+      <c r="H106" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J106" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="X106">
+        <v>1</v>
+      </c>
+      <c r="AE106" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF106">
+        <v>6</v>
+      </c>
+      <c r="AG106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="B107" t="s">
+        <v>5</v>
+      </c>
+      <c r="C107">
+        <v>7</v>
+      </c>
+      <c r="I107" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K107" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE107" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF107">
+        <v>7</v>
+      </c>
+      <c r="AG107">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="B108" t="s">
+        <v>6</v>
+      </c>
+      <c r="C108">
+        <v>8</v>
+      </c>
+      <c r="J108" t="s">
+        <v>14</v>
+      </c>
+      <c r="K108" t="s">
+        <v>15</v>
+      </c>
+      <c r="L108" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M108" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AE108" t="s">
+        <v>6</v>
+      </c>
+      <c r="AF108">
+        <v>8</v>
+      </c>
+      <c r="AG108">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="B109" t="s">
+        <v>6</v>
+      </c>
+      <c r="C109">
+        <v>9</v>
+      </c>
+      <c r="L109" t="s">
+        <v>18</v>
+      </c>
+      <c r="M109">
+        <v>-1</v>
+      </c>
+      <c r="AE109" t="s">
+        <v>6</v>
+      </c>
+      <c r="AF109">
+        <v>9</v>
+      </c>
+      <c r="AG109" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="110" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="B110" t="s">
+        <v>7</v>
+      </c>
+      <c r="C110">
+        <v>10</v>
+      </c>
+      <c r="J110" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L110" t="s">
+        <v>20</v>
+      </c>
+      <c r="N110" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE110" t="s">
+        <v>7</v>
+      </c>
+      <c r="AF110">
+        <v>10</v>
+      </c>
+      <c r="AG110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="B111" t="s">
+        <v>7</v>
+      </c>
+      <c r="C111">
+        <v>11</v>
+      </c>
+      <c r="K111" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M111" t="s">
+        <v>22</v>
+      </c>
+      <c r="O111" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE111" t="s">
+        <v>7</v>
+      </c>
+      <c r="AF111">
+        <v>11</v>
+      </c>
+      <c r="AG111">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="B112" t="s">
+        <v>8</v>
+      </c>
+      <c r="C112">
+        <v>12</v>
+      </c>
+      <c r="N112" t="s">
+        <v>0</v>
+      </c>
+      <c r="P112" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y112">
+        <v>1</v>
+      </c>
+      <c r="AE112" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF112">
+        <v>12</v>
+      </c>
+      <c r="AG112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="B113" t="s">
+        <v>8</v>
+      </c>
+      <c r="C113">
+        <v>13</v>
+      </c>
+      <c r="O113" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q113" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE113" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF113">
+        <v>13</v>
+      </c>
+      <c r="AG113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="B114" t="s">
+        <v>9</v>
+      </c>
+      <c r="C114">
+        <v>14</v>
+      </c>
+      <c r="P114" t="s">
+        <v>0</v>
+      </c>
+      <c r="R114" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z114">
+        <v>1</v>
+      </c>
+      <c r="AE114" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF114">
+        <v>14</v>
+      </c>
+      <c r="AG114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="B115" t="s">
+        <v>9</v>
+      </c>
+      <c r="C115">
+        <v>15</v>
+      </c>
+      <c r="Q115" t="s">
+        <v>3</v>
+      </c>
+      <c r="S115" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA115">
+        <v>1</v>
+      </c>
+      <c r="AE115" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF115">
+        <v>15</v>
+      </c>
+      <c r="AG115">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="B116" t="s">
+        <v>10</v>
+      </c>
+      <c r="C116">
+        <v>16</v>
+      </c>
+      <c r="R116" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z116">
+        <v>1</v>
+      </c>
+      <c r="AE116" t="s">
+        <v>10</v>
+      </c>
+      <c r="AF116">
+        <v>16</v>
+      </c>
+      <c r="AG116" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="117" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="B117" t="s">
+        <v>10</v>
+      </c>
+      <c r="C117">
+        <v>17</v>
+      </c>
+      <c r="S117" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA117">
+        <v>1</v>
+      </c>
+      <c r="AE117" t="s">
+        <v>10</v>
+      </c>
+      <c r="AF117">
+        <v>17</v>
+      </c>
+      <c r="AG117" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="118" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="B118" t="s">
+        <v>11</v>
+      </c>
+      <c r="C118">
+        <v>18</v>
+      </c>
+      <c r="R118" t="s">
+        <v>26</v>
+      </c>
+      <c r="X118">
+        <v>1</v>
+      </c>
+      <c r="AE118" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF118">
+        <v>18</v>
+      </c>
+      <c r="AG118" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="119" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="B119" t="s">
+        <v>11</v>
+      </c>
+      <c r="C119">
+        <v>19</v>
+      </c>
+      <c r="S119" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y119">
+        <v>1</v>
+      </c>
+      <c r="AE119" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF119">
+        <v>19</v>
+      </c>
+      <c r="AG119" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="120" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="B120" t="s">
+        <v>64</v>
+      </c>
+      <c r="C120">
+        <v>20</v>
+      </c>
+      <c r="R120" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="T120" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AC120" s="7">
+        <v>-1</v>
+      </c>
+      <c r="AE120" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF120">
+        <v>20</v>
+      </c>
+      <c r="AG120">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="B121" t="s">
+        <v>64</v>
+      </c>
+      <c r="C121">
+        <v>21</v>
+      </c>
+      <c r="S121" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="T121" s="7"/>
+      <c r="U121" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="V121" s="7"/>
+      <c r="W121" s="7"/>
+      <c r="X121" s="7"/>
+      <c r="Y121" s="7"/>
+      <c r="Z121" s="7"/>
+      <c r="AA121" s="7"/>
+      <c r="AB121" s="7"/>
+      <c r="AC121" s="7"/>
+      <c r="AD121" s="7">
+        <v>-1</v>
+      </c>
+      <c r="AE121" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF121">
+        <v>21</v>
+      </c>
+      <c r="AG121">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="B122" t="s">
+        <v>65</v>
+      </c>
+      <c r="C122">
+        <v>22</v>
+      </c>
+      <c r="R122" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="S122" s="7"/>
+      <c r="T122" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="U122" s="7"/>
+      <c r="V122" s="7">
+        <v>-1</v>
+      </c>
+      <c r="W122" s="7"/>
+      <c r="X122" s="7"/>
+      <c r="Y122" s="7"/>
+      <c r="Z122" s="7"/>
+      <c r="AA122" s="7"/>
+      <c r="AB122" s="7"/>
+      <c r="AC122" s="7"/>
+      <c r="AD122" s="7"/>
+      <c r="AE122" t="s">
+        <v>65</v>
+      </c>
+      <c r="AF122">
+        <v>22</v>
+      </c>
+      <c r="AG122">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="B123" t="s">
+        <v>65</v>
+      </c>
+      <c r="C123">
+        <v>23</v>
+      </c>
+      <c r="S123" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="T123" s="7"/>
+      <c r="U123" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="V123" s="7"/>
+      <c r="W123" s="7">
+        <v>-1</v>
+      </c>
+      <c r="X123" s="7"/>
+      <c r="Y123" s="7"/>
+      <c r="Z123" s="7"/>
+      <c r="AA123" s="7"/>
+      <c r="AB123" s="7"/>
+      <c r="AC123" s="7"/>
+      <c r="AD123" s="7"/>
+      <c r="AE123" t="s">
+        <v>65</v>
+      </c>
+      <c r="AF123">
+        <v>23</v>
+      </c>
+      <c r="AG123">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="B124" t="s">
+        <v>99</v>
+      </c>
+      <c r="C124">
+        <v>24</v>
+      </c>
+      <c r="D124" t="s">
+        <v>92</v>
+      </c>
+      <c r="R124" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="S124" s="7"/>
+      <c r="T124" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="U124" s="7"/>
+      <c r="V124" s="7"/>
+      <c r="W124" s="7"/>
+      <c r="X124" s="7"/>
+      <c r="Y124" s="7"/>
+      <c r="Z124" s="7"/>
+      <c r="AA124" s="7"/>
+      <c r="AB124" s="7"/>
+      <c r="AC124" s="7">
+        <v>2</v>
+      </c>
+      <c r="AD124" s="7">
+        <v>2</v>
+      </c>
+      <c r="AE124" t="s">
+        <v>99</v>
+      </c>
+      <c r="AF124">
+        <v>24</v>
+      </c>
+      <c r="AG124" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="125" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="B125" t="s">
+        <v>99</v>
+      </c>
+      <c r="C125">
+        <v>25</v>
+      </c>
+      <c r="S125" s="7"/>
+      <c r="T125" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="U125" s="7">
+        <v>-1</v>
+      </c>
+      <c r="V125" s="7"/>
+      <c r="W125" s="7"/>
+      <c r="X125" s="7"/>
+      <c r="Y125" s="7"/>
+      <c r="Z125" s="7"/>
+      <c r="AA125" s="7"/>
+      <c r="AB125" s="7"/>
+      <c r="AC125" s="7"/>
+      <c r="AD125" s="7"/>
+      <c r="AE125" t="s">
+        <v>99</v>
+      </c>
+      <c r="AF125">
+        <v>25</v>
+      </c>
+      <c r="AG125" s="7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="126" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="B126" t="s">
+        <v>99</v>
+      </c>
+      <c r="C126">
+        <v>26</v>
+      </c>
+      <c r="AB126">
+        <v>1</v>
+      </c>
+      <c r="AC126">
+        <v>-1</v>
+      </c>
+      <c r="AD126">
+        <v>-1</v>
+      </c>
+      <c r="AE126" t="s">
+        <v>99</v>
+      </c>
+      <c r="AF126">
+        <v>26</v>
+      </c>
+      <c r="AG126">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="C127" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D127" t="s">
+        <v>39</v>
+      </c>
+      <c r="E127" t="s">
+        <v>40</v>
+      </c>
+      <c r="F127" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G127" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H127" t="s">
+        <v>43</v>
+      </c>
+      <c r="I127" t="s">
+        <v>44</v>
+      </c>
+      <c r="J127" t="s">
+        <v>45</v>
+      </c>
+      <c r="K127" t="s">
+        <v>46</v>
+      </c>
+      <c r="L127" t="s">
+        <v>47</v>
+      </c>
+      <c r="M127" t="s">
+        <v>48</v>
+      </c>
+      <c r="N127" t="s">
+        <v>49</v>
+      </c>
+      <c r="O127" t="s">
+        <v>50</v>
+      </c>
+      <c r="P127" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q127" t="s">
+        <v>56</v>
+      </c>
+      <c r="R127" t="s">
+        <v>60</v>
+      </c>
+      <c r="S127" t="s">
+        <v>61</v>
+      </c>
+      <c r="T127" t="s">
+        <v>83</v>
+      </c>
+      <c r="U127" t="s">
+        <v>84</v>
+      </c>
+      <c r="V127" t="s">
+        <v>85</v>
+      </c>
+      <c r="W127" t="s">
+        <v>86</v>
+      </c>
+      <c r="X127" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y127" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z127" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA127" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB127" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC127" t="s">
+        <v>72</v>
+      </c>
+      <c r="AD127" t="s">
+        <v>71</v>
+      </c>
+      <c r="AF127" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="132" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="C132" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D132">
+        <v>0</v>
+      </c>
+      <c r="E132">
+        <v>1</v>
+      </c>
+      <c r="F132">
+        <v>2</v>
+      </c>
+      <c r="G132">
+        <v>3</v>
+      </c>
+      <c r="H132">
+        <v>4</v>
+      </c>
+      <c r="I132">
+        <v>5</v>
+      </c>
+      <c r="J132">
+        <v>6</v>
+      </c>
+      <c r="K132">
+        <v>7</v>
+      </c>
+      <c r="L132">
+        <v>8</v>
+      </c>
+      <c r="M132">
+        <v>9</v>
+      </c>
+      <c r="N132">
+        <v>10</v>
+      </c>
+      <c r="O132">
+        <v>11</v>
+      </c>
+      <c r="P132">
+        <v>12</v>
+      </c>
+      <c r="Q132">
+        <v>13</v>
+      </c>
+      <c r="R132">
+        <v>14</v>
+      </c>
+      <c r="S132">
+        <v>15</v>
+      </c>
+      <c r="T132">
+        <v>16</v>
+      </c>
+      <c r="U132">
+        <v>17</v>
+      </c>
+      <c r="V132">
+        <v>18</v>
+      </c>
+      <c r="W132">
+        <v>19</v>
+      </c>
+      <c r="X132">
+        <v>20</v>
+      </c>
+      <c r="Y132">
+        <v>21</v>
+      </c>
+      <c r="Z132">
+        <v>22</v>
+      </c>
+      <c r="AA132">
+        <v>23</v>
+      </c>
+      <c r="AB132">
+        <v>24</v>
+      </c>
+      <c r="AC132">
+        <v>25</v>
+      </c>
+      <c r="AD132">
+        <v>26</v>
+      </c>
+      <c r="AG132" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="133" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="B133" t="s">
+        <v>63</v>
+      </c>
+      <c r="C133">
+        <v>0</v>
+      </c>
+      <c r="D133" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB133">
+        <v>1</v>
+      </c>
+      <c r="AE133" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF133">
+        <v>0</v>
+      </c>
+      <c r="AG133" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="134" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="B134" t="s">
+        <v>63</v>
+      </c>
+      <c r="C134">
+        <v>1</v>
+      </c>
+      <c r="E134">
+        <v>1</v>
+      </c>
+      <c r="AE134" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF134">
+        <v>1</v>
+      </c>
+      <c r="AG134" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="135" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="B135" t="s">
+        <v>1</v>
+      </c>
+      <c r="C135">
+        <v>2</v>
+      </c>
+      <c r="D135" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F135" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R135" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="AE135" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF135">
+        <v>2</v>
+      </c>
+      <c r="AG135">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="B136" t="s">
+        <v>1</v>
+      </c>
+      <c r="C136">
+        <v>3</v>
+      </c>
+      <c r="E136" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G136" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="S136" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="AE136" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF136">
+        <v>3</v>
+      </c>
+      <c r="AG136">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="B137" t="s">
+        <v>5</v>
+      </c>
+      <c r="C137">
+        <v>4</v>
+      </c>
+      <c r="F137" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H137" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="X137">
+        <v>1</v>
+      </c>
+      <c r="AE137" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF137">
+        <v>4</v>
+      </c>
+      <c r="AG137">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="B138" t="s">
+        <v>5</v>
+      </c>
+      <c r="C138">
+        <v>5</v>
+      </c>
+      <c r="G138" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I138" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE138" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF138">
+        <v>5</v>
+      </c>
+      <c r="AG138">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="B139" t="s">
+        <v>6</v>
+      </c>
+      <c r="C139">
+        <v>6</v>
+      </c>
+      <c r="H139" t="s">
+        <v>14</v>
+      </c>
+      <c r="I139" t="s">
+        <v>15</v>
+      </c>
+      <c r="J139" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K139" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AE139" t="s">
+        <v>6</v>
+      </c>
+      <c r="AF139">
+        <v>6</v>
+      </c>
+      <c r="AG139">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="B140" t="s">
+        <v>6</v>
+      </c>
+      <c r="C140">
+        <v>7</v>
+      </c>
+      <c r="J140" t="s">
+        <v>18</v>
+      </c>
+      <c r="K140">
+        <v>-1</v>
+      </c>
+      <c r="AE140" t="s">
+        <v>6</v>
+      </c>
+      <c r="AF140">
+        <v>7</v>
+      </c>
+      <c r="AG140" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="141" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="B141" t="s">
+        <v>7</v>
+      </c>
+      <c r="C141">
+        <v>8</v>
+      </c>
+      <c r="H141" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J141" t="s">
+        <v>20</v>
+      </c>
+      <c r="L141" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE141" t="s">
+        <v>7</v>
+      </c>
+      <c r="AF141">
+        <v>8</v>
+      </c>
+      <c r="AG141">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="B142" t="s">
+        <v>7</v>
+      </c>
+      <c r="C142">
+        <v>9</v>
+      </c>
+      <c r="I142" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K142" t="s">
+        <v>22</v>
+      </c>
+      <c r="M142" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE142" t="s">
+        <v>7</v>
+      </c>
+      <c r="AF142">
+        <v>9</v>
+      </c>
+      <c r="AG142">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="B143" t="s">
+        <v>27</v>
+      </c>
+      <c r="C143">
+        <v>10</v>
+      </c>
+      <c r="L143" t="s">
+        <v>14</v>
+      </c>
+      <c r="M143" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N143" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O143" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AE143" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF143">
+        <v>10</v>
+      </c>
+      <c r="AG143">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="B144" t="s">
+        <v>27</v>
+      </c>
+      <c r="C144">
+        <v>11</v>
+      </c>
+      <c r="M144" s="1"/>
+      <c r="N144" t="s">
+        <v>57</v>
+      </c>
+      <c r="O144">
+        <v>-1</v>
+      </c>
+      <c r="AE144" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF144">
+        <v>11</v>
+      </c>
+      <c r="AG144" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="145" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="B145" t="s">
+        <v>8</v>
+      </c>
+      <c r="C145">
+        <v>12</v>
+      </c>
+      <c r="N145" t="s">
+        <v>0</v>
+      </c>
+      <c r="P145" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y145">
+        <v>1</v>
+      </c>
+      <c r="AE145" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF145">
+        <v>12</v>
+      </c>
+      <c r="AG145">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="B146" t="s">
+        <v>8</v>
+      </c>
+      <c r="C146">
+        <v>13</v>
+      </c>
+      <c r="O146" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q146" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE146" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF146">
+        <v>13</v>
+      </c>
+      <c r="AG146">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="B147" t="s">
+        <v>9</v>
+      </c>
+      <c r="C147">
+        <v>14</v>
+      </c>
+      <c r="P147" t="s">
+        <v>0</v>
+      </c>
+      <c r="R147" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z147">
+        <v>1</v>
+      </c>
+      <c r="AE147" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF147">
+        <v>14</v>
+      </c>
+      <c r="AG147">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="B148" t="s">
+        <v>9</v>
+      </c>
+      <c r="C148">
+        <v>15</v>
+      </c>
+      <c r="Q148" t="s">
+        <v>3</v>
+      </c>
+      <c r="S148" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA148">
+        <v>1</v>
+      </c>
+      <c r="AE148" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF148">
+        <v>15</v>
+      </c>
+      <c r="AG148">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="B149" t="s">
+        <v>10</v>
+      </c>
+      <c r="C149">
+        <v>16</v>
+      </c>
+      <c r="R149" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z149">
+        <v>1</v>
+      </c>
+      <c r="AE149" t="s">
+        <v>10</v>
+      </c>
+      <c r="AF149">
+        <v>16</v>
+      </c>
+      <c r="AG149" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="150" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="B150" t="s">
+        <v>10</v>
+      </c>
+      <c r="C150">
+        <v>17</v>
+      </c>
+      <c r="S150" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA150">
+        <v>1</v>
+      </c>
+      <c r="AE150" t="s">
+        <v>10</v>
+      </c>
+      <c r="AF150">
+        <v>17</v>
+      </c>
+      <c r="AG150" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="151" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="B151" t="s">
+        <v>11</v>
+      </c>
+      <c r="C151">
+        <v>18</v>
+      </c>
+      <c r="R151" t="s">
+        <v>26</v>
+      </c>
+      <c r="X151">
+        <v>1</v>
+      </c>
+      <c r="AE151" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF151">
+        <v>18</v>
+      </c>
+      <c r="AG151" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="152" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="B152" t="s">
+        <v>11</v>
+      </c>
+      <c r="C152">
+        <v>19</v>
+      </c>
+      <c r="S152" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y152">
+        <v>1</v>
+      </c>
+      <c r="AE152" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF152">
+        <v>19</v>
+      </c>
+      <c r="AG152" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="153" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="B153" t="s">
+        <v>64</v>
+      </c>
+      <c r="C153">
+        <v>20</v>
+      </c>
+      <c r="R153" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="T153" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AC153" s="7">
+        <v>-1</v>
+      </c>
+      <c r="AE153" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF153">
+        <v>20</v>
+      </c>
+      <c r="AG153">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="B154" t="s">
+        <v>64</v>
+      </c>
+      <c r="C154">
+        <v>21</v>
+      </c>
+      <c r="S154" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="T154" s="7"/>
+      <c r="U154" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="V154" s="7"/>
+      <c r="W154" s="7"/>
+      <c r="X154" s="7"/>
+      <c r="Y154" s="7"/>
+      <c r="Z154" s="7"/>
+      <c r="AA154" s="7"/>
+      <c r="AB154" s="7"/>
+      <c r="AC154" s="7"/>
+      <c r="AD154" s="7">
+        <v>-1</v>
+      </c>
+      <c r="AE154" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF154">
+        <v>21</v>
+      </c>
+      <c r="AG154">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="B155" t="s">
+        <v>65</v>
+      </c>
+      <c r="C155">
+        <v>22</v>
+      </c>
+      <c r="R155" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="S155" s="7"/>
+      <c r="T155" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="U155" s="7"/>
+      <c r="V155" s="7">
+        <v>-1</v>
+      </c>
+      <c r="W155" s="7"/>
+      <c r="X155" s="7"/>
+      <c r="Y155" s="7"/>
+      <c r="Z155" s="7"/>
+      <c r="AA155" s="7"/>
+      <c r="AB155" s="7"/>
+      <c r="AC155" s="7"/>
+      <c r="AD155" s="7"/>
+      <c r="AE155" t="s">
+        <v>65</v>
+      </c>
+      <c r="AF155">
+        <v>22</v>
+      </c>
+      <c r="AG155">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="B156" t="s">
+        <v>65</v>
+      </c>
+      <c r="C156">
+        <v>23</v>
+      </c>
+      <c r="S156" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="T156" s="7"/>
+      <c r="U156" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="V156" s="7"/>
+      <c r="W156" s="7">
+        <v>-1</v>
+      </c>
+      <c r="X156" s="7"/>
+      <c r="Y156" s="7"/>
+      <c r="Z156" s="7"/>
+      <c r="AA156" s="7"/>
+      <c r="AB156" s="7"/>
+      <c r="AC156" s="7"/>
+      <c r="AD156" s="7"/>
+      <c r="AE156" t="s">
+        <v>65</v>
+      </c>
+      <c r="AF156">
+        <v>23</v>
+      </c>
+      <c r="AG156">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="B157" t="s">
+        <v>99</v>
+      </c>
+      <c r="C157">
+        <v>24</v>
+      </c>
+      <c r="D157" t="s">
+        <v>92</v>
+      </c>
+      <c r="R157" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="S157" s="7"/>
+      <c r="T157" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="U157" s="7"/>
+      <c r="V157" s="7"/>
+      <c r="W157" s="7"/>
+      <c r="X157" s="7"/>
+      <c r="Y157" s="7"/>
+      <c r="Z157" s="7"/>
+      <c r="AA157" s="7"/>
+      <c r="AB157" s="7"/>
+      <c r="AC157" s="7">
+        <v>2</v>
+      </c>
+      <c r="AD157" s="7">
+        <v>2</v>
+      </c>
+      <c r="AE157" t="s">
+        <v>99</v>
+      </c>
+      <c r="AF157">
+        <v>24</v>
+      </c>
+      <c r="AG157" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="158" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="B158" t="s">
+        <v>99</v>
+      </c>
+      <c r="C158">
+        <v>25</v>
+      </c>
+      <c r="S158" s="7"/>
+      <c r="T158" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="U158" s="7">
+        <v>-1</v>
+      </c>
+      <c r="V158" s="7"/>
+      <c r="W158" s="7"/>
+      <c r="X158" s="7"/>
+      <c r="Y158" s="7"/>
+      <c r="Z158" s="7"/>
+      <c r="AA158" s="7"/>
+      <c r="AB158" s="7"/>
+      <c r="AC158" s="7"/>
+      <c r="AD158" s="7"/>
+      <c r="AE158" t="s">
+        <v>99</v>
+      </c>
+      <c r="AF158">
+        <v>25</v>
+      </c>
+      <c r="AG158" s="7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="159" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="B159" t="s">
+        <v>99</v>
+      </c>
+      <c r="C159">
+        <v>26</v>
+      </c>
+      <c r="AB159">
+        <v>1</v>
+      </c>
+      <c r="AC159">
+        <v>-1</v>
+      </c>
+      <c r="AD159">
+        <v>-1</v>
+      </c>
+      <c r="AE159" t="s">
+        <v>99</v>
+      </c>
+      <c r="AF159">
+        <v>26</v>
+      </c>
+      <c r="AG159">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="C160" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D160" t="s">
+        <v>39</v>
+      </c>
+      <c r="E160" t="s">
+        <v>40</v>
+      </c>
+      <c r="F160" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="G160" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="H160" t="s">
+        <v>43</v>
+      </c>
+      <c r="I160" t="s">
+        <v>44</v>
+      </c>
+      <c r="J160" t="s">
+        <v>45</v>
+      </c>
+      <c r="K160" t="s">
+        <v>46</v>
+      </c>
+      <c r="L160" t="s">
+        <v>47</v>
+      </c>
+      <c r="M160" t="s">
+        <v>48</v>
+      </c>
+      <c r="N160" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="O160" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="P160" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q160" t="s">
+        <v>56</v>
+      </c>
+      <c r="R160" t="s">
+        <v>60</v>
+      </c>
+      <c r="S160" t="s">
+        <v>61</v>
+      </c>
+      <c r="T160" t="s">
+        <v>83</v>
+      </c>
+      <c r="U160" t="s">
+        <v>84</v>
+      </c>
+      <c r="V160" t="s">
+        <v>85</v>
+      </c>
+      <c r="W160" t="s">
+        <v>86</v>
+      </c>
+      <c r="X160" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y160" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z160" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA160" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB160" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC160" t="s">
+        <v>72</v>
+      </c>
+      <c r="AD160" t="s">
+        <v>71</v>
+      </c>
+      <c r="AF160" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="165" spans="2:35" x14ac:dyDescent="0.3">
+      <c r="C165" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="D165">
+        <v>0</v>
+      </c>
+      <c r="E165">
+        <v>1</v>
+      </c>
+      <c r="F165">
+        <v>2</v>
+      </c>
+      <c r="G165">
+        <v>3</v>
+      </c>
+      <c r="H165">
+        <v>4</v>
+      </c>
+      <c r="I165">
+        <v>5</v>
+      </c>
+      <c r="J165">
+        <v>6</v>
+      </c>
+      <c r="K165">
+        <v>7</v>
+      </c>
+      <c r="L165">
+        <v>8</v>
+      </c>
+      <c r="M165">
+        <v>9</v>
+      </c>
+      <c r="N165">
+        <v>10</v>
+      </c>
+      <c r="O165">
+        <v>11</v>
+      </c>
+      <c r="P165">
+        <v>12</v>
+      </c>
+      <c r="Q165">
+        <v>13</v>
+      </c>
+      <c r="R165">
+        <v>14</v>
+      </c>
+      <c r="S165">
+        <v>15</v>
+      </c>
+      <c r="T165">
+        <v>16</v>
+      </c>
+      <c r="U165">
+        <v>17</v>
+      </c>
+      <c r="V165">
+        <v>18</v>
+      </c>
+      <c r="W165">
+        <v>19</v>
+      </c>
+      <c r="X165">
+        <v>20</v>
+      </c>
+      <c r="Y165">
+        <v>21</v>
+      </c>
+      <c r="Z165">
+        <v>22</v>
+      </c>
+      <c r="AA165">
+        <v>23</v>
+      </c>
+      <c r="AB165">
+        <v>24</v>
+      </c>
+      <c r="AC165">
+        <v>25</v>
+      </c>
+      <c r="AD165">
+        <v>26</v>
+      </c>
+      <c r="AE165">
+        <v>27</v>
+      </c>
+      <c r="AF165">
+        <v>28</v>
+      </c>
+      <c r="AI165" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="166" spans="2:35" x14ac:dyDescent="0.3">
+      <c r="B166" t="s">
+        <v>63</v>
+      </c>
+      <c r="C166">
+        <v>0</v>
+      </c>
+      <c r="D166" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AD166">
+        <v>1</v>
+      </c>
+      <c r="AG166" t="s">
+        <v>63</v>
+      </c>
+      <c r="AH166">
+        <v>0</v>
+      </c>
+      <c r="AI166" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="167" spans="2:35" x14ac:dyDescent="0.3">
+      <c r="B167" t="s">
+        <v>63</v>
+      </c>
+      <c r="C167">
+        <v>1</v>
+      </c>
+      <c r="E167">
+        <v>1</v>
+      </c>
+      <c r="AG167" t="s">
+        <v>63</v>
+      </c>
+      <c r="AH167">
+        <v>1</v>
+      </c>
+      <c r="AI167" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="168" spans="2:35" x14ac:dyDescent="0.3">
+      <c r="B168" t="s">
+        <v>1</v>
+      </c>
+      <c r="C168">
+        <v>2</v>
+      </c>
+      <c r="D168" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F168" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="T168" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="AG168" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH168">
+        <v>2</v>
+      </c>
+      <c r="AI168">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="2:35" x14ac:dyDescent="0.3">
+      <c r="B169" t="s">
+        <v>1</v>
+      </c>
+      <c r="C169">
+        <v>3</v>
+      </c>
+      <c r="E169" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G169" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="U169" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="AG169" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH169">
+        <v>3</v>
+      </c>
+      <c r="AI169">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" spans="2:35" x14ac:dyDescent="0.3">
+      <c r="B170" t="s">
+        <v>59</v>
+      </c>
+      <c r="C170">
+        <v>4</v>
+      </c>
+      <c r="F170" t="s">
+        <v>14</v>
+      </c>
+      <c r="G170" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H170" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I170" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AG170" t="s">
+        <v>59</v>
+      </c>
+      <c r="AH170">
+        <v>4</v>
+      </c>
+      <c r="AI170">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="2:35" x14ac:dyDescent="0.3">
+      <c r="B171" t="s">
+        <v>59</v>
+      </c>
+      <c r="C171">
+        <v>5</v>
+      </c>
+      <c r="G171" s="1"/>
+      <c r="H171" t="s">
+        <v>57</v>
+      </c>
+      <c r="I171">
+        <v>-1</v>
+      </c>
+      <c r="AG171" t="s">
+        <v>59</v>
+      </c>
+      <c r="AH171">
+        <v>5</v>
+      </c>
+      <c r="AI171" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="172" spans="2:35" x14ac:dyDescent="0.3">
+      <c r="B172" t="s">
+        <v>5</v>
+      </c>
+      <c r="C172">
+        <v>6</v>
+      </c>
+      <c r="H172" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J172" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z172">
+        <v>1</v>
+      </c>
+      <c r="AG172" t="s">
+        <v>5</v>
+      </c>
+      <c r="AH172">
+        <v>6</v>
+      </c>
+      <c r="AI172">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="2:35" x14ac:dyDescent="0.3">
+      <c r="B173" t="s">
+        <v>5</v>
+      </c>
+      <c r="C173">
+        <v>7</v>
+      </c>
+      <c r="I173" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K173" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AG173" t="s">
+        <v>5</v>
+      </c>
+      <c r="AH173">
+        <v>7</v>
+      </c>
+      <c r="AI173">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="2:35" x14ac:dyDescent="0.3">
+      <c r="B174" t="s">
+        <v>6</v>
+      </c>
+      <c r="C174">
+        <v>8</v>
+      </c>
+      <c r="J174" t="s">
+        <v>14</v>
+      </c>
+      <c r="K174" t="s">
+        <v>15</v>
+      </c>
+      <c r="L174" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M174" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AG174" t="s">
+        <v>6</v>
+      </c>
+      <c r="AH174">
+        <v>8</v>
+      </c>
+      <c r="AI174">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="2:35" x14ac:dyDescent="0.3">
+      <c r="B175" t="s">
+        <v>6</v>
+      </c>
+      <c r="C175">
+        <v>9</v>
+      </c>
+      <c r="L175" t="s">
+        <v>18</v>
+      </c>
+      <c r="M175">
+        <v>-1</v>
+      </c>
+      <c r="AG175" t="s">
+        <v>6</v>
+      </c>
+      <c r="AH175">
+        <v>9</v>
+      </c>
+      <c r="AI175" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="176" spans="2:35" x14ac:dyDescent="0.3">
+      <c r="B176" t="s">
+        <v>7</v>
+      </c>
+      <c r="C176">
+        <v>10</v>
+      </c>
+      <c r="J176" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L176" t="s">
+        <v>20</v>
+      </c>
+      <c r="N176" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG176" t="s">
+        <v>7</v>
+      </c>
+      <c r="AH176">
+        <v>10</v>
+      </c>
+      <c r="AI176">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="2:35" x14ac:dyDescent="0.3">
+      <c r="B177" t="s">
+        <v>7</v>
+      </c>
+      <c r="C177">
+        <v>11</v>
+      </c>
+      <c r="K177" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M177" t="s">
+        <v>22</v>
+      </c>
+      <c r="O177" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AG177" t="s">
+        <v>7</v>
+      </c>
+      <c r="AH177">
+        <v>11</v>
+      </c>
+      <c r="AI177">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="2:35" x14ac:dyDescent="0.3">
+      <c r="B178" t="s">
+        <v>27</v>
+      </c>
+      <c r="C178">
+        <v>12</v>
+      </c>
+      <c r="N178" t="s">
+        <v>14</v>
+      </c>
+      <c r="O178" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P178" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q178" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AG178" t="s">
+        <v>27</v>
+      </c>
+      <c r="AH178">
+        <v>12</v>
+      </c>
+      <c r="AI178">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="2:35" x14ac:dyDescent="0.3">
+      <c r="B179" t="s">
+        <v>27</v>
+      </c>
+      <c r="C179">
+        <v>13</v>
+      </c>
+      <c r="O179" s="1"/>
+      <c r="P179" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q179">
+        <v>-1</v>
+      </c>
+      <c r="AG179" t="s">
+        <v>27</v>
+      </c>
+      <c r="AH179">
+        <v>13</v>
+      </c>
+      <c r="AI179" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="180" spans="2:35" x14ac:dyDescent="0.3">
+      <c r="B180" t="s">
+        <v>8</v>
+      </c>
+      <c r="C180">
+        <v>14</v>
+      </c>
+      <c r="P180" t="s">
+        <v>0</v>
+      </c>
+      <c r="R180" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA180">
+        <v>1</v>
+      </c>
+      <c r="AG180" t="s">
+        <v>8</v>
+      </c>
+      <c r="AH180">
+        <v>14</v>
+      </c>
+      <c r="AI180">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="2:35" x14ac:dyDescent="0.3">
+      <c r="B181" t="s">
+        <v>8</v>
+      </c>
+      <c r="C181">
+        <v>15</v>
+      </c>
+      <c r="Q181" t="s">
+        <v>3</v>
+      </c>
+      <c r="S181" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AG181" t="s">
+        <v>8</v>
+      </c>
+      <c r="AH181">
+        <v>15</v>
+      </c>
+      <c r="AI181">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182" spans="2:35" x14ac:dyDescent="0.3">
+      <c r="B182" t="s">
+        <v>9</v>
+      </c>
+      <c r="C182">
+        <v>16</v>
+      </c>
+      <c r="R182" t="s">
+        <v>0</v>
+      </c>
+      <c r="T182" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB182">
+        <v>1</v>
+      </c>
+      <c r="AG182" t="s">
+        <v>9</v>
+      </c>
+      <c r="AH182">
+        <v>16</v>
+      </c>
+      <c r="AI182">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183" spans="2:35" x14ac:dyDescent="0.3">
+      <c r="B183" t="s">
+        <v>9</v>
+      </c>
+      <c r="C183">
+        <v>17</v>
+      </c>
+      <c r="S183" t="s">
+        <v>3</v>
+      </c>
+      <c r="U183" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC183">
+        <v>1</v>
+      </c>
+      <c r="AG183" t="s">
+        <v>9</v>
+      </c>
+      <c r="AH183">
+        <v>17</v>
+      </c>
+      <c r="AI183">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184" spans="2:35" x14ac:dyDescent="0.3">
+      <c r="B184" t="s">
+        <v>10</v>
+      </c>
+      <c r="C184">
+        <v>18</v>
+      </c>
+      <c r="T184" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB184">
+        <v>1</v>
+      </c>
+      <c r="AG184" t="s">
+        <v>10</v>
+      </c>
+      <c r="AH184">
+        <v>18</v>
+      </c>
+      <c r="AI184" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="185" spans="2:35" x14ac:dyDescent="0.3">
+      <c r="B185" t="s">
+        <v>10</v>
+      </c>
+      <c r="C185">
+        <v>19</v>
+      </c>
+      <c r="U185" t="s">
+        <v>24</v>
+      </c>
+      <c r="AC185">
+        <v>1</v>
+      </c>
+      <c r="AG185" t="s">
+        <v>10</v>
+      </c>
+      <c r="AH185">
+        <v>19</v>
+      </c>
+      <c r="AI185" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="186" spans="2:35" x14ac:dyDescent="0.3">
+      <c r="B186" t="s">
+        <v>11</v>
+      </c>
+      <c r="C186">
+        <v>20</v>
+      </c>
+      <c r="T186" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z186">
+        <v>1</v>
+      </c>
+      <c r="AG186" t="s">
+        <v>11</v>
+      </c>
+      <c r="AH186">
+        <v>20</v>
+      </c>
+      <c r="AI186" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="187" spans="2:35" x14ac:dyDescent="0.3">
+      <c r="B187" t="s">
+        <v>11</v>
+      </c>
+      <c r="C187">
+        <v>21</v>
+      </c>
+      <c r="U187" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA187">
+        <v>1</v>
+      </c>
+      <c r="AG187" t="s">
+        <v>11</v>
+      </c>
+      <c r="AH187">
+        <v>21</v>
+      </c>
+      <c r="AI187" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="188" spans="2:35" x14ac:dyDescent="0.3">
+      <c r="B188" t="s">
+        <v>64</v>
+      </c>
+      <c r="C188">
+        <v>22</v>
+      </c>
+      <c r="T188" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="V188" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AE188" s="7">
+        <v>-1</v>
+      </c>
+      <c r="AG188" t="s">
+        <v>64</v>
+      </c>
+      <c r="AH188">
+        <v>22</v>
+      </c>
+      <c r="AI188">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="189" spans="2:35" x14ac:dyDescent="0.3">
+      <c r="B189" t="s">
+        <v>64</v>
+      </c>
+      <c r="C189">
+        <v>23</v>
+      </c>
+      <c r="U189" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="V189" s="7"/>
+      <c r="W189" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="X189" s="7"/>
+      <c r="Y189" s="7"/>
+      <c r="Z189" s="7"/>
+      <c r="AA189" s="7"/>
+      <c r="AB189" s="7"/>
+      <c r="AC189" s="7"/>
+      <c r="AD189" s="7"/>
+      <c r="AE189" s="7"/>
+      <c r="AF189" s="7">
+        <v>-1</v>
+      </c>
+      <c r="AG189" t="s">
+        <v>64</v>
+      </c>
+      <c r="AH189">
+        <v>23</v>
+      </c>
+      <c r="AI189">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190" spans="2:35" x14ac:dyDescent="0.3">
+      <c r="B190" t="s">
+        <v>65</v>
+      </c>
+      <c r="C190">
+        <v>24</v>
+      </c>
+      <c r="T190" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="U190" s="7"/>
+      <c r="V190" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="W190" s="7"/>
+      <c r="X190" s="7">
+        <v>-1</v>
+      </c>
+      <c r="Y190" s="7"/>
+      <c r="Z190" s="7"/>
+      <c r="AA190" s="7"/>
+      <c r="AB190" s="7"/>
+      <c r="AC190" s="7"/>
+      <c r="AD190" s="7"/>
+      <c r="AE190" s="7"/>
+      <c r="AF190" s="7"/>
+      <c r="AG190" t="s">
+        <v>65</v>
+      </c>
+      <c r="AH190">
+        <v>24</v>
+      </c>
+      <c r="AI190">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" spans="2:35" x14ac:dyDescent="0.3">
+      <c r="B191" t="s">
+        <v>65</v>
+      </c>
+      <c r="C191">
+        <v>25</v>
+      </c>
+      <c r="U191" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="V191" s="7"/>
+      <c r="W191" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="X191" s="7"/>
+      <c r="Y191" s="7">
+        <v>-1</v>
+      </c>
+      <c r="Z191" s="7"/>
+      <c r="AA191" s="7"/>
+      <c r="AB191" s="7"/>
+      <c r="AC191" s="7"/>
+      <c r="AD191" s="7"/>
+      <c r="AE191" s="7"/>
+      <c r="AF191" s="7"/>
+      <c r="AG191" t="s">
+        <v>65</v>
+      </c>
+      <c r="AH191">
+        <v>25</v>
+      </c>
+      <c r="AI191">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192" spans="2:35" x14ac:dyDescent="0.3">
+      <c r="B192" t="s">
+        <v>99</v>
+      </c>
+      <c r="C192">
+        <v>26</v>
+      </c>
+      <c r="D192" t="s">
+        <v>92</v>
+      </c>
+      <c r="T192" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="U192" s="7"/>
+      <c r="V192" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="W192" s="7"/>
+      <c r="X192" s="7"/>
+      <c r="Y192" s="7"/>
+      <c r="Z192" s="7"/>
+      <c r="AA192" s="7"/>
+      <c r="AB192" s="7"/>
+      <c r="AC192" s="7"/>
+      <c r="AD192" s="7"/>
+      <c r="AE192" s="7">
+        <v>2</v>
+      </c>
+      <c r="AF192" s="7">
+        <v>2</v>
+      </c>
+      <c r="AG192" t="s">
+        <v>99</v>
+      </c>
+      <c r="AH192">
+        <v>26</v>
+      </c>
+      <c r="AI192" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="193" spans="2:35" x14ac:dyDescent="0.3">
+      <c r="B193" t="s">
+        <v>99</v>
+      </c>
+      <c r="C193">
+        <v>27</v>
+      </c>
+      <c r="U193" s="7"/>
+      <c r="V193" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="W193" s="7">
+        <v>-1</v>
+      </c>
+      <c r="X193" s="7"/>
+      <c r="Y193" s="7"/>
+      <c r="Z193" s="7"/>
+      <c r="AA193" s="7"/>
+      <c r="AB193" s="7"/>
+      <c r="AC193" s="7"/>
+      <c r="AD193" s="7"/>
+      <c r="AE193" s="7"/>
+      <c r="AF193" s="7"/>
+      <c r="AG193" t="s">
+        <v>99</v>
+      </c>
+      <c r="AH193">
+        <v>27</v>
+      </c>
+      <c r="AI193" s="7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="194" spans="2:35" x14ac:dyDescent="0.3">
+      <c r="B194" t="s">
+        <v>99</v>
+      </c>
+      <c r="C194">
+        <v>28</v>
+      </c>
+      <c r="AD194">
+        <v>1</v>
+      </c>
+      <c r="AE194">
+        <v>-1</v>
+      </c>
+      <c r="AF194">
+        <v>-1</v>
+      </c>
+      <c r="AG194" t="s">
+        <v>99</v>
+      </c>
+      <c r="AH194">
+        <v>28</v>
+      </c>
+      <c r="AI194">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195" spans="2:35" x14ac:dyDescent="0.3">
+      <c r="C195" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D195" t="s">
+        <v>39</v>
+      </c>
+      <c r="E195" t="s">
+        <v>40</v>
+      </c>
+      <c r="F195" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G195" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H195" t="s">
+        <v>43</v>
+      </c>
+      <c r="I195" t="s">
+        <v>44</v>
+      </c>
+      <c r="J195" t="s">
+        <v>45</v>
+      </c>
+      <c r="K195" t="s">
+        <v>46</v>
+      </c>
+      <c r="L195" t="s">
+        <v>47</v>
+      </c>
+      <c r="M195" t="s">
+        <v>48</v>
+      </c>
+      <c r="N195" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="O195" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="P195" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q195" t="s">
+        <v>56</v>
+      </c>
+      <c r="R195" t="s">
+        <v>60</v>
+      </c>
+      <c r="S195" t="s">
+        <v>61</v>
+      </c>
+      <c r="T195" t="s">
+        <v>83</v>
+      </c>
+      <c r="U195" t="s">
+        <v>84</v>
+      </c>
+      <c r="V195" t="s">
+        <v>85</v>
+      </c>
+      <c r="W195" t="s">
+        <v>86</v>
+      </c>
+      <c r="X195" t="s">
+        <v>115</v>
+      </c>
+      <c r="Y195" t="s">
+        <v>116</v>
+      </c>
+      <c r="Z195" t="s">
+        <v>51</v>
+      </c>
+      <c r="AA195" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB195" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC195" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD195" t="s">
+        <v>67</v>
+      </c>
+      <c r="AE195" t="s">
+        <v>72</v>
+      </c>
+      <c r="AF195" t="s">
+        <v>71</v>
+      </c>
+      <c r="AG195" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>